<commit_message>
400 x 4 is last?
</commit_message>
<xml_diff>
--- a/timings.xlsx
+++ b/timings.xlsx
@@ -158,7 +158,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -195,6 +195,9 @@
       <c r="C3" s="1" t="n">
         <v>0.000296</v>
       </c>
+      <c r="D3" s="1" t="n">
+        <v>0.00183</v>
+      </c>
       <c r="E3" s="1" t="n">
         <v>0.007393</v>
       </c>
@@ -209,6 +212,9 @@
       <c r="C4" s="1" t="n">
         <v>0.002277</v>
       </c>
+      <c r="D4" s="1" t="n">
+        <v>0.54</v>
+      </c>
       <c r="E4" s="1" t="n">
         <v>28</v>
       </c>
@@ -222,6 +228,9 @@
       </c>
       <c r="C5" s="1" t="n">
         <v>0.037</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>